<commit_message>
inserindo legenda no grafico
</commit_message>
<xml_diff>
--- a/dados_diabete.xlsx
+++ b/dados_diabete.xlsx
@@ -370,13 +370,14 @@
   </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.18"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>